<commit_message>
added Rizika file (first draft of Hladina)
</commit_message>
<xml_diff>
--- a/Dokumentace a přílohy/Rizika.xlsx
+++ b/Dokumentace a přílohy/Rizika.xlsx
@@ -1,25 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asher\Desktop\Škola\4 Sem\RSP\Dev\rsproject\Dokumentace a přílohy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA157A07-CB97-4538-B01E-3F89C23FB4F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5220" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Rizika</t>
+  </si>
+  <si>
+    <t>Název</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Popis</t>
+  </si>
+  <si>
+    <t>Pravděpodobnost</t>
+  </si>
+  <si>
+    <t>Závažnost</t>
+  </si>
+  <si>
+    <t>Prevence</t>
+  </si>
+  <si>
+    <t>Řešení</t>
+  </si>
+  <si>
+    <t>Zodpovědný člověk</t>
+  </si>
+  <si>
+    <t>Hladina</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +377,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <f>(E4+10*F4)/2</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J16" si="0">(E5+10*F5)/2</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>99</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Functional and nonFunctional requirements and Risks
</commit_message>
<xml_diff>
--- a/Dokumentace a přílohy/Rizika.xlsx
+++ b/Dokumentace a přílohy/Rizika.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asher\Desktop\Škola\4 Sem\RSP\Dev\rsproject\Dokumentace a přílohy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA157A07-CB97-4538-B01E-3F89C23FB4F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9E7DCB-A15A-407B-BFE8-8658D2275867}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5565" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Rizika</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Popis</t>
   </si>
   <si>
-    <t>Pravděpodobnost</t>
-  </si>
-  <si>
-    <t>Závažnost</t>
-  </si>
-  <si>
     <t>Prevence</t>
   </si>
   <si>
@@ -61,16 +55,64 @@
   </si>
   <si>
     <t>Hladina</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Pravděpodobnost*</t>
+  </si>
+  <si>
+    <t>Závažnost**</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>udáváno v procentech</t>
+  </si>
+  <si>
+    <t>škála 1 - 10 (deset je nejvíc)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,19 +420,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J16"/>
+  <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
@@ -409,97 +454,91 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E4">
-        <v>90</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
       </c>
       <c r="J4">
         <f>(E4+10*F4)/2</f>
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5:J16" si="0">(E5+10*F5)/2</f>
-        <v>52.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>99</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>54.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <v>50</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
       <c r="J9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
       <c r="J10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
       <c r="J11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -535,7 +574,24 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>